<commit_message>
Effort Commitment up to date
</commit_message>
<xml_diff>
--- a/documentation/budget/effort_commitment.xlsx
+++ b/documentation/budget/effort_commitment.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26122"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-7000" yWindow="-28500" windowWidth="48580" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="42640" yWindow="-10320" windowWidth="36440" windowHeight="20660" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -547,7 +547,7 @@
     <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="134">
+  <dxfs count="52">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -665,826 +665,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2218,7 +1398,7 @@
   <dimension ref="B1:AG47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="M30" sqref="M30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2408,17 +1588,17 @@
         <v>21</v>
       </c>
       <c r="D15" s="2">
-        <v>2017</v>
+        <v>2019</v>
       </c>
       <c r="E15" s="2">
         <v>10</v>
       </c>
       <c r="F15" s="2">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="G15" s="4">
         <f>DATE($D$15,$E$15,$F$15)</f>
-        <v>43031</v>
+        <v>43752</v>
       </c>
     </row>
     <row r="17" spans="2:32">
@@ -2514,7 +1694,7 @@
         <v>27</v>
       </c>
       <c r="M20" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="N20" s="2" t="s">
         <v>28</v>
@@ -2523,7 +1703,7 @@
         <v>28</v>
       </c>
       <c r="P20" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="Q20" s="2" t="s">
         <v>27</v>
@@ -2647,7 +1827,7 @@
         <v>1.75</v>
       </c>
       <c r="I22" s="5">
-        <f t="shared" ref="H22:Z22" si="0">(+I21 + 0.5)/2</f>
+        <f t="shared" ref="I22:Y22" si="0">(+I21 + 0.5)/2</f>
         <v>2.75</v>
       </c>
       <c r="K22" s="5">
@@ -2688,92 +1868,92 @@
         <v>20</v>
       </c>
       <c r="E23" s="4">
-        <f>$G$15 +($C$2  * (E$21-1))</f>
-        <v>43031</v>
+        <f t="shared" ref="E23:Z23" si="1">$G$15 +($C$2  * (E$21-1))</f>
+        <v>43752</v>
       </c>
       <c r="F23" s="4">
-        <f>$G$15 +($C$2  * (F$21-1))</f>
-        <v>43038</v>
+        <f t="shared" si="1"/>
+        <v>43759</v>
       </c>
       <c r="G23" s="4">
-        <f>$G$15 +($C$2  * (G$21-1))</f>
-        <v>43045</v>
+        <f t="shared" si="1"/>
+        <v>43766</v>
       </c>
       <c r="H23" s="4">
-        <f>$G$15 +($C$2  * (H$21-1))</f>
-        <v>43052</v>
+        <f t="shared" si="1"/>
+        <v>43773</v>
       </c>
       <c r="I23" s="4">
-        <f>$G$15 +($C$2  * (I$21-1))</f>
-        <v>43059</v>
+        <f t="shared" si="1"/>
+        <v>43780</v>
       </c>
       <c r="J23" s="4">
-        <f>$G$15 +($C$2  * (J$21-1))</f>
-        <v>43066</v>
+        <f t="shared" si="1"/>
+        <v>43787</v>
       </c>
       <c r="K23" s="4">
-        <f>$G$15 +($C$2  * (K$21-1))</f>
-        <v>43073</v>
+        <f t="shared" si="1"/>
+        <v>43794</v>
       </c>
       <c r="L23" s="4">
-        <f>$G$15 +($C$2  * (L$21-1))</f>
-        <v>43080</v>
+        <f t="shared" si="1"/>
+        <v>43801</v>
       </c>
       <c r="M23" s="4">
-        <f>$G$15 +($C$2  * (M$21-1))</f>
-        <v>43087</v>
+        <f t="shared" si="1"/>
+        <v>43808</v>
       </c>
       <c r="N23" s="4">
-        <f>$G$15 +($C$2  * (N$21-1))</f>
-        <v>43094</v>
+        <f t="shared" si="1"/>
+        <v>43815</v>
       </c>
       <c r="O23" s="4">
-        <f>$G$15 +($C$2  * (O$21-1))</f>
-        <v>43101</v>
+        <f t="shared" si="1"/>
+        <v>43822</v>
       </c>
       <c r="P23" s="4">
-        <f>$G$15 +($C$2  * (P$21-1))</f>
-        <v>43108</v>
+        <f t="shared" si="1"/>
+        <v>43829</v>
       </c>
       <c r="Q23" s="4">
-        <f>$G$15 +($C$2  * (Q$21-1))</f>
-        <v>43115</v>
+        <f t="shared" si="1"/>
+        <v>43836</v>
       </c>
       <c r="R23" s="4">
-        <f>$G$15 +($C$2  * (R$21-1))</f>
-        <v>43122</v>
+        <f t="shared" si="1"/>
+        <v>43843</v>
       </c>
       <c r="S23" s="4">
-        <f>$G$15 +($C$2  * (S$21-1))</f>
-        <v>43129</v>
+        <f t="shared" si="1"/>
+        <v>43850</v>
       </c>
       <c r="T23" s="4">
-        <f>$G$15 +($C$2  * (T$21-1))</f>
-        <v>43136</v>
+        <f t="shared" si="1"/>
+        <v>43857</v>
       </c>
       <c r="U23" s="4">
-        <f>$G$15 +($C$2  * (U$21-1))</f>
-        <v>43143</v>
+        <f t="shared" si="1"/>
+        <v>43864</v>
       </c>
       <c r="V23" s="4">
-        <f>$G$15 +($C$2  * (V$21-1))</f>
-        <v>43150</v>
+        <f t="shared" si="1"/>
+        <v>43871</v>
       </c>
       <c r="W23" s="4">
-        <f>$G$15 +($C$2  * (W$21-1))</f>
-        <v>43157</v>
+        <f t="shared" si="1"/>
+        <v>43878</v>
       </c>
       <c r="X23" s="4">
-        <f>$G$15 +($C$2  * (X$21-1))</f>
-        <v>43164</v>
+        <f t="shared" si="1"/>
+        <v>43885</v>
       </c>
       <c r="Y23" s="4">
-        <f>$G$15 +($C$2  * (Y$21-1))</f>
-        <v>43171</v>
+        <f t="shared" si="1"/>
+        <v>43892</v>
       </c>
       <c r="Z23" s="4">
-        <f>$G$15 +($C$2  * (Z$21-1))</f>
-        <v>43178</v>
+        <f t="shared" si="1"/>
+        <v>43899</v>
       </c>
       <c r="AC23" s="5" t="str">
         <f>$I$9</f>
@@ -2820,7 +2000,7 @@
         <v>12</v>
       </c>
       <c r="M24" s="14" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="N24" s="14" t="s">
         <v>31</v>
@@ -2829,7 +2009,7 @@
         <v>31</v>
       </c>
       <c r="P24" s="14" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="Q24" s="14" t="s">
         <v>12</v>
@@ -2862,19 +2042,19 @@
         <v>12</v>
       </c>
       <c r="AC24" s="3">
-        <f>COUNTIFS($E24:$AB24,$I$9) * $F$9</f>
+        <f t="shared" ref="AC24:AC33" si="2">COUNTIFS($E24:$AB24,$I$9) * $F$9</f>
         <v>96.662500000000009</v>
       </c>
       <c r="AD24" s="3">
-        <f>COUNTIFS($E24:$AB24,$I$10) * $F$10</f>
+        <f t="shared" ref="AD24:AD33" si="3">COUNTIFS($E24:$AB24,$I$10) * $F$10</f>
         <v>0</v>
       </c>
       <c r="AE24" s="3">
-        <f>COUNTIFS($E24:$AB24,$I$11) * $F$11</f>
+        <f t="shared" ref="AE24:AE33" si="4">COUNTIFS($E24:$AB24,$I$11) * $F$11</f>
         <v>0</v>
       </c>
       <c r="AF24" s="3">
-        <f>SUM(AC24:AE24)</f>
+        <f t="shared" ref="AF24:AF33" si="5">SUM(AC24:AE24)</f>
         <v>96.662500000000009</v>
       </c>
     </row>
@@ -2907,7 +2087,7 @@
         <v>12</v>
       </c>
       <c r="M25" s="9" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="N25" s="9" t="s">
         <v>31</v>
@@ -2916,7 +2096,7 @@
         <v>31</v>
       </c>
       <c r="P25" s="9" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="Q25" s="9" t="s">
         <v>12</v>
@@ -2949,19 +2129,19 @@
         <v>12</v>
       </c>
       <c r="AC25" s="3">
-        <f>COUNTIFS($E25:$AB25,$I$9) * $F$9</f>
+        <f t="shared" si="2"/>
         <v>96.662500000000009</v>
       </c>
       <c r="AD25" s="3">
-        <f>COUNTIFS($E25:$AB25,$I$10) * $F$10</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AE25" s="3">
-        <f>COUNTIFS($E25:$AB25,$I$11) * $F$11</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AF25" s="3">
-        <f>SUM(AC25:AE25)</f>
+        <f t="shared" si="5"/>
         <v>96.662500000000009</v>
       </c>
     </row>
@@ -2994,7 +2174,7 @@
         <v>12</v>
       </c>
       <c r="M26" s="9" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="N26" s="9" t="s">
         <v>31</v>
@@ -3003,7 +2183,7 @@
         <v>31</v>
       </c>
       <c r="P26" s="9" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="Q26" s="9" t="s">
         <v>12</v>
@@ -3036,19 +2216,19 @@
         <v>12</v>
       </c>
       <c r="AC26" s="3">
-        <f>COUNTIFS($E26:$AB26,$I$9) * $F$9</f>
+        <f t="shared" si="2"/>
         <v>96.662500000000009</v>
       </c>
       <c r="AD26" s="3">
-        <f>COUNTIFS($E26:$AB26,$I$10) * $F$10</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AE26" s="3">
-        <f>COUNTIFS($E26:$AB26,$I$11) * $F$11</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AF26" s="3">
-        <f>SUM(AC26:AE26)</f>
+        <f t="shared" si="5"/>
         <v>96.662500000000009</v>
       </c>
     </row>
@@ -3081,7 +2261,7 @@
         <v>12</v>
       </c>
       <c r="M27" s="9" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="N27" s="9" t="s">
         <v>31</v>
@@ -3090,7 +2270,7 @@
         <v>31</v>
       </c>
       <c r="P27" s="9" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="Q27" s="9" t="s">
         <v>12</v>
@@ -3123,19 +2303,19 @@
         <v>12</v>
       </c>
       <c r="AC27" s="3">
-        <f>COUNTIFS($E27:$AB27,$I$9) * $F$9</f>
+        <f t="shared" si="2"/>
         <v>96.662500000000009</v>
       </c>
       <c r="AD27" s="3">
-        <f>COUNTIFS($E27:$AB27,$I$10) * $F$10</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AE27" s="3">
-        <f>COUNTIFS($E27:$AB27,$I$11) * $F$11</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AF27" s="3">
-        <f>SUM(AC27:AE27)</f>
+        <f t="shared" si="5"/>
         <v>96.662500000000009</v>
       </c>
     </row>
@@ -3210,19 +2390,19 @@
         <v>31</v>
       </c>
       <c r="AC28" s="3">
-        <f>COUNTIFS($E28:$AB28,$I$9) * $F$9</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AD28" s="3">
-        <f>COUNTIFS($E28:$AB28,$I$10) * $F$10</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AE28" s="3">
-        <f>COUNTIFS($E28:$AB28,$I$11) * $F$11</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AF28" s="3">
-        <f>SUM(AC28:AE28)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -3297,19 +2477,19 @@
         <v>31</v>
       </c>
       <c r="AC29" s="3">
-        <f>COUNTIFS($E29:$AB29,$I$9) * $F$9</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AD29" s="3">
-        <f>COUNTIFS($E29:$AB29,$I$10) * $F$10</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AE29" s="3">
-        <f>COUNTIFS($E29:$AB29,$I$11) * $F$11</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AF29" s="3">
-        <f>SUM(AC29:AE29)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -3384,19 +2564,19 @@
         <v>31</v>
       </c>
       <c r="AC30" s="3">
-        <f>COUNTIFS($E30:$AB30,$I$9) * $F$9</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AD30" s="3">
-        <f>COUNTIFS($E30:$AB30,$I$10) * $F$10</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AE30" s="3">
-        <f>COUNTIFS($E30:$AB30,$I$11) * $F$11</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AF30" s="3">
-        <f>SUM(AC30:AE30)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -3471,19 +2651,19 @@
         <v>31</v>
       </c>
       <c r="AC31" s="3">
-        <f>COUNTIFS($E31:$AB31,$I$9) * $F$9</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AD31" s="3">
-        <f>COUNTIFS($E31:$AB31,$I$10) * $F$10</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AE31" s="3">
-        <f>COUNTIFS($E31:$AB31,$I$11) * $F$11</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AF31" s="3">
-        <f>SUM(AC31:AE31)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -3558,19 +2738,19 @@
         <v>31</v>
       </c>
       <c r="AC32" s="3">
-        <f>COUNTIFS($E32:$AB32,$I$9) * $F$9</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AD32" s="3">
-        <f>COUNTIFS($E32:$AB32,$I$10) * $F$10</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AE32" s="3">
-        <f>COUNTIFS($E32:$AB32,$I$11) * $F$11</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AF32" s="3">
-        <f>SUM(AC32:AE32)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -3645,19 +2825,19 @@
         <v>31</v>
       </c>
       <c r="AC33" s="3">
-        <f>COUNTIFS($E33:$AB33,$I$9) * $F$9</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AD33" s="3">
-        <f>COUNTIFS($E33:$AB33,$I$10) * $F$10</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AE33" s="3">
-        <f>COUNTIFS($E33:$AB33,$I$11) * $F$11</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AF33" s="3">
-        <f>SUM(AC33:AE33)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -3673,91 +2853,91 @@
         <v>Minimum</v>
       </c>
       <c r="E35" s="3">
-        <f>COUNTIFS(E$24:E$34,$I9) * $F$9</f>
+        <f t="shared" ref="E35:Z35" si="6">COUNTIFS(E$24:E$34,$I9) * $F$9</f>
         <v>20.350000000000001</v>
       </c>
       <c r="F35" s="3">
-        <f>COUNTIFS(F$24:F$34,$I9) * $F$9</f>
+        <f t="shared" si="6"/>
         <v>20.350000000000001</v>
       </c>
       <c r="G35" s="3">
-        <f>COUNTIFS(G$24:G$34,$I9) * $F$9</f>
+        <f t="shared" si="6"/>
         <v>20.350000000000001</v>
       </c>
       <c r="H35" s="3">
-        <f>COUNTIFS(H$24:H$34,$I9) * $F$9</f>
+        <f t="shared" si="6"/>
         <v>20.350000000000001</v>
       </c>
       <c r="I35" s="3">
-        <f>COUNTIFS(I$24:I$34,$I9) * $F$9</f>
+        <f t="shared" si="6"/>
         <v>20.350000000000001</v>
       </c>
       <c r="J35" s="3">
-        <f>COUNTIFS(J$24:J$34,$I9) * $F$9</f>
+        <f t="shared" si="6"/>
         <v>20.350000000000001</v>
       </c>
       <c r="K35" s="3">
-        <f>COUNTIFS(K$24:K$34,$I9) * $F$9</f>
+        <f t="shared" si="6"/>
         <v>20.350000000000001</v>
       </c>
       <c r="L35" s="3">
-        <f>COUNTIFS(L$24:L$34,$I9) * $F$9</f>
+        <f t="shared" si="6"/>
         <v>20.350000000000001</v>
       </c>
       <c r="M35" s="3">
-        <f>COUNTIFS(M$24:M$34,$I9) * $F$9</f>
-        <v>0</v>
+        <f t="shared" si="6"/>
+        <v>20.350000000000001</v>
       </c>
       <c r="N35" s="3">
-        <f>COUNTIFS(N$24:N$34,$I9) * $F$9</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="O35" s="3">
-        <f>COUNTIFS(O$24:O$34,$I9) * $F$9</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="P35" s="3">
-        <f>COUNTIFS(P$24:P$34,$I9) * $F$9</f>
-        <v>20.350000000000001</v>
+        <f t="shared" si="6"/>
+        <v>0</v>
       </c>
       <c r="Q35" s="3">
-        <f>COUNTIFS(Q$24:Q$34,$I9) * $F$9</f>
+        <f t="shared" si="6"/>
         <v>20.350000000000001</v>
       </c>
       <c r="R35" s="3">
-        <f>COUNTIFS(R$24:R$34,$I9) * $F$9</f>
+        <f t="shared" si="6"/>
         <v>20.350000000000001</v>
       </c>
       <c r="S35" s="3">
-        <f>COUNTIFS(S$24:S$34,$I9) * $F$9</f>
+        <f t="shared" si="6"/>
         <v>20.350000000000001</v>
       </c>
       <c r="T35" s="3">
-        <f>COUNTIFS(T$24:T$34,$I9) * $F$9</f>
+        <f t="shared" si="6"/>
         <v>20.350000000000001</v>
       </c>
       <c r="U35" s="3">
-        <f>COUNTIFS(U$24:U$34,$I9) * $F$9</f>
+        <f t="shared" si="6"/>
         <v>20.350000000000001</v>
       </c>
       <c r="V35" s="3">
-        <f>COUNTIFS(V$24:V$34,$I9) * $F$9</f>
+        <f t="shared" si="6"/>
         <v>20.350000000000001</v>
       </c>
       <c r="W35" s="3">
-        <f>COUNTIFS(W$24:W$34,$I9) * $F$9</f>
+        <f t="shared" si="6"/>
         <v>20.350000000000001</v>
       </c>
       <c r="X35" s="3">
-        <f>COUNTIFS(X$24:X$34,$I9) * $F$9</f>
+        <f t="shared" si="6"/>
         <v>20.350000000000001</v>
       </c>
       <c r="Y35" s="3">
-        <f>COUNTIFS(Y$24:Y$34,$I9) * $F$9</f>
+        <f t="shared" si="6"/>
         <v>20.350000000000001</v>
       </c>
       <c r="Z35" s="3">
-        <f>COUNTIFS(Z$24:Z$34,$I9) * $F$9</f>
+        <f t="shared" si="6"/>
         <v>20.350000000000001</v>
       </c>
     </row>
@@ -3768,91 +2948,91 @@
         <v>Expected</v>
       </c>
       <c r="E36" s="3">
-        <f>COUNTIFS(E$24:E$34,$I10) * $F$10</f>
+        <f t="shared" ref="E36:Z36" si="7">COUNTIFS(E$24:E$34,$I10) * $F$10</f>
         <v>0</v>
       </c>
       <c r="F36" s="3">
-        <f>COUNTIFS(F$24:F$34,$I10) * $F$10</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="G36" s="3">
-        <f>COUNTIFS(G$24:G$34,$I10) * $F$10</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H36" s="3">
-        <f>COUNTIFS(H$24:H$34,$I10) * $F$10</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="I36" s="3">
-        <f>COUNTIFS(I$24:I$34,$I10) * $F$10</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="J36" s="3">
-        <f>COUNTIFS(J$24:J$34,$I10) * $F$10</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="K36" s="3">
-        <f>COUNTIFS(K$24:K$34,$I10) * $F$10</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="L36" s="3">
-        <f>COUNTIFS(L$24:L$34,$I10) * $F$10</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="M36" s="3">
-        <f>COUNTIFS(M$24:M$34,$I10) * $F$10</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="N36" s="3">
-        <f>COUNTIFS(N$24:N$34,$I10) * $F$10</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="O36" s="3">
-        <f>COUNTIFS(O$24:O$34,$I10) * $F$10</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="P36" s="3">
-        <f>COUNTIFS(P$24:P$34,$I10) * $F$10</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="Q36" s="3">
-        <f>COUNTIFS(Q$24:Q$34,$I10) * $F$10</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="R36" s="3">
-        <f>COUNTIFS(R$24:R$34,$I10) * $F$10</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="S36" s="3">
-        <f>COUNTIFS(S$24:S$34,$I10) * $F$10</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="T36" s="3">
-        <f>COUNTIFS(T$24:T$34,$I10) * $F$10</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="U36" s="3">
-        <f>COUNTIFS(U$24:U$34,$I10) * $F$10</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="V36" s="3">
-        <f>COUNTIFS(V$24:V$34,$I10) * $F$10</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="W36" s="3">
-        <f>COUNTIFS(W$24:W$34,$I10) * $F$10</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="X36" s="3">
-        <f>COUNTIFS(X$24:X$34,$I10) * $F$10</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="Y36" s="3">
-        <f>COUNTIFS(Y$24:Y$34,$I10) * $F$10</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="Z36" s="3">
-        <f>COUNTIFS(Z$24:Z$34,$I10) * $F$10</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AB36" s="5" t="s">
@@ -3885,91 +3065,91 @@
         <v>Stretch</v>
       </c>
       <c r="E37" s="3">
-        <f>COUNTIFS(E$24:E$34,$I11) * $F$11</f>
+        <f t="shared" ref="E37:Z37" si="8">COUNTIFS(E$24:E$34,$I11) * $F$11</f>
         <v>0</v>
       </c>
       <c r="F37" s="3">
-        <f>COUNTIFS(F$24:F$34,$I11) * $F$11</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="G37" s="3">
-        <f>COUNTIFS(G$24:G$34,$I11) * $F$11</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="H37" s="3">
-        <f>COUNTIFS(H$24:H$34,$I11) * $F$11</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="I37" s="3">
-        <f>COUNTIFS(I$24:I$34,$I11) * $F$11</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="J37" s="3">
-        <f>COUNTIFS(J$24:J$34,$I11) * $F$11</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="K37" s="3">
-        <f>COUNTIFS(K$24:K$34,$I11) * $F$11</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="L37" s="3">
-        <f>COUNTIFS(L$24:L$34,$I11) * $F$11</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="M37" s="3">
-        <f>COUNTIFS(M$24:M$34,$I11) * $F$11</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="N37" s="3">
-        <f>COUNTIFS(N$24:N$34,$I11) * $F$11</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="O37" s="3">
-        <f>COUNTIFS(O$24:O$34,$I11) * $F$11</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="P37" s="3">
-        <f>COUNTIFS(P$24:P$34,$I11) * $F$11</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="Q37" s="3">
-        <f>COUNTIFS(Q$24:Q$34,$I11) * $F$11</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="R37" s="3">
-        <f>COUNTIFS(R$24:R$34,$I11) * $F$11</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="S37" s="3">
-        <f>COUNTIFS(S$24:S$34,$I11) * $F$11</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="T37" s="3">
-        <f>COUNTIFS(T$24:T$34,$I11) * $F$11</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="U37" s="3">
-        <f>COUNTIFS(U$24:U$34,$I11) * $F$11</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="V37" s="3">
-        <f>COUNTIFS(V$24:V$34,$I11) * $F$11</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="W37" s="3">
-        <f>COUNTIFS(W$24:W$34,$I11) * $F$11</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="X37" s="3">
-        <f>COUNTIFS(X$24:X$34,$I11) * $F$11</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="Y37" s="3">
-        <f>COUNTIFS(Y$24:Y$34,$I11) * $F$11</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="Z37" s="3">
-        <f>COUNTIFS(Z$24:Z$34,$I11) * $F$11</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
@@ -3997,91 +3177,91 @@
         <v>19</v>
       </c>
       <c r="E42" s="3">
-        <f t="shared" ref="E42:Z42" si="1">SUM(E35:E37)</f>
+        <f t="shared" ref="E42:Z42" si="9">SUM(E35:E37)</f>
         <v>20.350000000000001</v>
       </c>
       <c r="F42" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>20.350000000000001</v>
       </c>
       <c r="G42" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>20.350000000000001</v>
       </c>
       <c r="H42" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>20.350000000000001</v>
       </c>
       <c r="I42" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>20.350000000000001</v>
       </c>
       <c r="J42" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>20.350000000000001</v>
       </c>
       <c r="K42" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>20.350000000000001</v>
       </c>
       <c r="L42" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>20.350000000000001</v>
       </c>
       <c r="M42" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="9"/>
+        <v>20.350000000000001</v>
       </c>
       <c r="N42" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="O42" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="P42" s="3">
-        <f t="shared" si="1"/>
-        <v>20.350000000000001</v>
+        <f t="shared" si="9"/>
+        <v>0</v>
       </c>
       <c r="Q42" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>20.350000000000001</v>
       </c>
       <c r="R42" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>20.350000000000001</v>
       </c>
       <c r="S42" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>20.350000000000001</v>
       </c>
       <c r="T42" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>20.350000000000001</v>
       </c>
       <c r="U42" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>20.350000000000001</v>
       </c>
       <c r="V42" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>20.350000000000001</v>
       </c>
       <c r="W42" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>20.350000000000001</v>
       </c>
       <c r="X42" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>20.350000000000001</v>
       </c>
       <c r="Y42" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>20.350000000000001</v>
       </c>
       <c r="Z42" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>20.350000000000001</v>
       </c>
       <c r="AB42" s="5" t="s">
@@ -4110,43 +3290,43 @@
         <v>40.700000000000003</v>
       </c>
       <c r="H43" s="3">
-        <f t="shared" ref="H43:Z43" si="2">SUM(G42:H42)</f>
+        <f t="shared" ref="H43:Z43" si="10">SUM(G42:H42)</f>
         <v>40.700000000000003</v>
       </c>
       <c r="J43" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>40.700000000000003</v>
       </c>
       <c r="L43" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>40.700000000000003</v>
       </c>
       <c r="N43" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" si="10"/>
+        <v>20.350000000000001</v>
       </c>
       <c r="P43" s="3">
-        <f t="shared" si="2"/>
-        <v>20.350000000000001</v>
+        <f t="shared" si="10"/>
+        <v>0</v>
       </c>
       <c r="R43" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>40.700000000000003</v>
       </c>
       <c r="T43" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>40.700000000000003</v>
       </c>
       <c r="V43" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>40.700000000000003</v>
       </c>
       <c r="X43" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>40.700000000000003</v>
       </c>
       <c r="Z43" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>40.700000000000003</v>
       </c>
       <c r="AB43" s="5" t="s">
@@ -4175,209 +3355,208 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <conditionalFormatting sqref="AF34:AF35 A32:B32 D32 AA32:XFD32">
-    <cfRule type="cellIs" dxfId="133" priority="132" operator="between">
+    <cfRule type="cellIs" dxfId="51" priority="132" operator="between">
       <formula>$I$11</formula>
       <formula>$I$11</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="132" priority="133" operator="between">
+    <cfRule type="cellIs" dxfId="50" priority="133" operator="between">
       <formula>$I$10</formula>
       <formula>$I$10</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="131" priority="134" operator="between">
+    <cfRule type="cellIs" dxfId="49" priority="134" operator="between">
       <formula>$I$9</formula>
       <formula>$I$9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A20:XFD20">
-    <cfRule type="cellIs" dxfId="130" priority="130" operator="between">
+    <cfRule type="cellIs" dxfId="48" priority="130" operator="between">
       <formula>$K$10</formula>
       <formula>$K$10</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="129" priority="131" operator="between">
+    <cfRule type="cellIs" dxfId="47" priority="131" operator="between">
       <formula>$K$9</formula>
       <formula>$K$9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E35:Z37">
-    <cfRule type="cellIs" dxfId="128" priority="127" operator="between">
+    <cfRule type="cellIs" dxfId="46" priority="127" operator="between">
       <formula>$I$11</formula>
       <formula>$I$11</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="127" priority="128" operator="between">
+    <cfRule type="cellIs" dxfId="45" priority="128" operator="between">
       <formula>$I$10</formula>
       <formula>$I$10</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="126" priority="129" operator="between">
+    <cfRule type="cellIs" dxfId="44" priority="129" operator="between">
       <formula>$I$9</formula>
       <formula>$I$9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A24:D24 C25:C32 AA24:XFD24">
-    <cfRule type="cellIs" dxfId="125" priority="124" operator="between">
+    <cfRule type="cellIs" dxfId="43" priority="124" operator="between">
       <formula>$I$11</formula>
       <formula>$I$11</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="124" priority="125" operator="between">
+    <cfRule type="cellIs" dxfId="42" priority="125" operator="between">
       <formula>$I$10</formula>
       <formula>$I$10</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="123" priority="126" operator="between">
+    <cfRule type="cellIs" dxfId="41" priority="126" operator="between">
       <formula>$I$9</formula>
       <formula>$I$9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A25:B25 D25 AA25:XFD25">
-    <cfRule type="cellIs" dxfId="122" priority="121" operator="between">
+    <cfRule type="cellIs" dxfId="40" priority="121" operator="between">
       <formula>$I$11</formula>
       <formula>$I$11</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="121" priority="122" operator="between">
+    <cfRule type="cellIs" dxfId="39" priority="122" operator="between">
       <formula>$I$10</formula>
       <formula>$I$10</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="120" priority="123" operator="between">
+    <cfRule type="cellIs" dxfId="38" priority="123" operator="between">
       <formula>$I$9</formula>
       <formula>$I$9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A26:B26 D26 AA26:XFD26">
-    <cfRule type="cellIs" dxfId="119" priority="118" operator="between">
+    <cfRule type="cellIs" dxfId="37" priority="118" operator="between">
       <formula>$I$11</formula>
       <formula>$I$11</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="118" priority="119" operator="between">
+    <cfRule type="cellIs" dxfId="36" priority="119" operator="between">
       <formula>$I$10</formula>
       <formula>$I$10</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="117" priority="120" operator="between">
+    <cfRule type="cellIs" dxfId="35" priority="120" operator="between">
       <formula>$I$9</formula>
       <formula>$I$9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A31:B31 D31 AA31:XFD31">
-    <cfRule type="cellIs" dxfId="116" priority="100" operator="between">
+    <cfRule type="cellIs" dxfId="34" priority="100" operator="between">
       <formula>$I$11</formula>
       <formula>$I$11</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="115" priority="101" operator="between">
+    <cfRule type="cellIs" dxfId="33" priority="101" operator="between">
       <formula>$I$10</formula>
       <formula>$I$10</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="114" priority="102" operator="between">
+    <cfRule type="cellIs" dxfId="32" priority="102" operator="between">
       <formula>$I$9</formula>
       <formula>$I$9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A27:B27 D27 AA27:XFD27">
-    <cfRule type="cellIs" dxfId="113" priority="112" operator="between">
+    <cfRule type="cellIs" dxfId="31" priority="112" operator="between">
       <formula>$I$11</formula>
       <formula>$I$11</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="112" priority="113" operator="between">
+    <cfRule type="cellIs" dxfId="30" priority="113" operator="between">
       <formula>$I$10</formula>
       <formula>$I$10</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="111" priority="114" operator="between">
+    <cfRule type="cellIs" dxfId="29" priority="114" operator="between">
       <formula>$I$9</formula>
       <formula>$I$9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A28:B28 D28 AA28:XFD28">
-    <cfRule type="cellIs" dxfId="110" priority="109" operator="between">
+    <cfRule type="cellIs" dxfId="28" priority="109" operator="between">
       <formula>$I$11</formula>
       <formula>$I$11</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="109" priority="110" operator="between">
+    <cfRule type="cellIs" dxfId="27" priority="110" operator="between">
       <formula>$I$10</formula>
       <formula>$I$10</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="108" priority="111" operator="between">
+    <cfRule type="cellIs" dxfId="26" priority="111" operator="between">
       <formula>$I$9</formula>
       <formula>$I$9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A29:B29 D29 AA29:XFD29">
-    <cfRule type="cellIs" dxfId="107" priority="106" operator="between">
+    <cfRule type="cellIs" dxfId="25" priority="106" operator="between">
       <formula>$I$11</formula>
       <formula>$I$11</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="106" priority="107" operator="between">
+    <cfRule type="cellIs" dxfId="24" priority="107" operator="between">
       <formula>$I$10</formula>
       <formula>$I$10</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="105" priority="108" operator="between">
+    <cfRule type="cellIs" dxfId="23" priority="108" operator="between">
       <formula>$I$9</formula>
       <formula>$I$9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A30:B30 D30 AA30:XFD30">
-    <cfRule type="cellIs" dxfId="104" priority="103" operator="between">
+    <cfRule type="cellIs" dxfId="22" priority="103" operator="between">
       <formula>$I$11</formula>
       <formula>$I$11</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="103" priority="104" operator="between">
+    <cfRule type="cellIs" dxfId="21" priority="104" operator="between">
       <formula>$I$10</formula>
       <formula>$I$10</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="102" priority="105" operator="between">
+    <cfRule type="cellIs" dxfId="20" priority="105" operator="between">
       <formula>$I$9</formula>
       <formula>$I$9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A33:B33 D33 AA33:XFD33">
-    <cfRule type="cellIs" dxfId="98" priority="97" operator="between">
+    <cfRule type="cellIs" dxfId="19" priority="97" operator="between">
       <formula>$I$11</formula>
       <formula>$I$11</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="97" priority="98" operator="between">
+    <cfRule type="cellIs" dxfId="18" priority="98" operator="between">
       <formula>$I$10</formula>
       <formula>$I$10</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="96" priority="99" operator="between">
+    <cfRule type="cellIs" dxfId="17" priority="99" operator="between">
       <formula>$I$9</formula>
       <formula>$I$9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C33">
-    <cfRule type="cellIs" dxfId="95" priority="94" operator="between">
+    <cfRule type="cellIs" dxfId="16" priority="94" operator="between">
       <formula>$I$11</formula>
       <formula>$I$11</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="94" priority="95" operator="between">
+    <cfRule type="cellIs" dxfId="15" priority="95" operator="between">
       <formula>$I$10</formula>
       <formula>$I$10</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="93" priority="96" operator="between">
+    <cfRule type="cellIs" dxfId="14" priority="96" operator="between">
       <formula>$I$9</formula>
       <formula>$I$9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P24:Z27">
-    <cfRule type="cellIs" dxfId="83" priority="82" operator="between">
+    <cfRule type="cellIs" dxfId="8" priority="82" operator="between">
       <formula>$I$11</formula>
       <formula>$I$11</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="82" priority="83" operator="between">
+    <cfRule type="cellIs" dxfId="7" priority="83" operator="between">
       <formula>$I$10</formula>
       <formula>$I$10</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="81" priority="84" operator="between">
+    <cfRule type="cellIs" dxfId="6" priority="84" operator="between">
       <formula>$I$9</formula>
       <formula>$I$9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E28:Z33 E24:O27">
-    <cfRule type="cellIs" dxfId="2" priority="43" operator="between">
+    <cfRule type="cellIs" dxfId="11" priority="43" operator="between">
       <formula>$I$11</formula>
       <formula>$I$11</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="44" operator="between">
+    <cfRule type="cellIs" dxfId="10" priority="44" operator="between">
       <formula>$I$10</formula>
       <formula>$I$10</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="45" operator="between">
+    <cfRule type="cellIs" dxfId="9" priority="45" operator="between">
       <formula>$I$9</formula>
       <formula>$I$9</formula>
     </cfRule>

</xml_diff>

<commit_message>
Corrected Sprint 1 date
</commit_message>
<xml_diff>
--- a/documentation/budget/effort_commitment.xlsx
+++ b/documentation/budget/effort_commitment.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26122"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="42640" yWindow="-10320" windowWidth="36440" windowHeight="20660" tabRatio="500"/>
+    <workbookView xWindow="35360" yWindow="-9280" windowWidth="46780" windowHeight="20520" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -547,7 +547,7 @@
     <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="52">
+  <dxfs count="44">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -585,86 +585,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1398,7 +1318,7 @@
   <dimension ref="B1:AG47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M30" sqref="M30"/>
+      <selection activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1594,11 +1514,11 @@
         <v>10</v>
       </c>
       <c r="F15" s="2">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="G15" s="4">
         <f>DATE($D$15,$E$15,$F$15)</f>
-        <v>43752</v>
+        <v>43766</v>
       </c>
     </row>
     <row r="17" spans="2:32">
@@ -1869,91 +1789,91 @@
       </c>
       <c r="E23" s="4">
         <f t="shared" ref="E23:Z23" si="1">$G$15 +($C$2  * (E$21-1))</f>
-        <v>43752</v>
+        <v>43766</v>
       </c>
       <c r="F23" s="4">
         <f t="shared" si="1"/>
-        <v>43759</v>
+        <v>43773</v>
       </c>
       <c r="G23" s="4">
         <f t="shared" si="1"/>
-        <v>43766</v>
+        <v>43780</v>
       </c>
       <c r="H23" s="4">
         <f t="shared" si="1"/>
-        <v>43773</v>
+        <v>43787</v>
       </c>
       <c r="I23" s="4">
         <f t="shared" si="1"/>
-        <v>43780</v>
+        <v>43794</v>
       </c>
       <c r="J23" s="4">
         <f t="shared" si="1"/>
-        <v>43787</v>
+        <v>43801</v>
       </c>
       <c r="K23" s="4">
         <f t="shared" si="1"/>
-        <v>43794</v>
+        <v>43808</v>
       </c>
       <c r="L23" s="4">
         <f t="shared" si="1"/>
-        <v>43801</v>
+        <v>43815</v>
       </c>
       <c r="M23" s="4">
         <f t="shared" si="1"/>
-        <v>43808</v>
+        <v>43822</v>
       </c>
       <c r="N23" s="4">
         <f t="shared" si="1"/>
-        <v>43815</v>
+        <v>43829</v>
       </c>
       <c r="O23" s="4">
         <f t="shared" si="1"/>
-        <v>43822</v>
+        <v>43836</v>
       </c>
       <c r="P23" s="4">
         <f t="shared" si="1"/>
-        <v>43829</v>
+        <v>43843</v>
       </c>
       <c r="Q23" s="4">
         <f t="shared" si="1"/>
-        <v>43836</v>
+        <v>43850</v>
       </c>
       <c r="R23" s="4">
         <f t="shared" si="1"/>
-        <v>43843</v>
+        <v>43857</v>
       </c>
       <c r="S23" s="4">
         <f t="shared" si="1"/>
-        <v>43850</v>
+        <v>43864</v>
       </c>
       <c r="T23" s="4">
         <f t="shared" si="1"/>
-        <v>43857</v>
+        <v>43871</v>
       </c>
       <c r="U23" s="4">
         <f t="shared" si="1"/>
-        <v>43864</v>
+        <v>43878</v>
       </c>
       <c r="V23" s="4">
         <f t="shared" si="1"/>
-        <v>43871</v>
+        <v>43885</v>
       </c>
       <c r="W23" s="4">
         <f t="shared" si="1"/>
-        <v>43878</v>
+        <v>43892</v>
       </c>
       <c r="X23" s="4">
         <f t="shared" si="1"/>
-        <v>43885</v>
+        <v>43899</v>
       </c>
       <c r="Y23" s="4">
         <f t="shared" si="1"/>
-        <v>43892</v>
+        <v>43906</v>
       </c>
       <c r="Z23" s="4">
         <f t="shared" si="1"/>
-        <v>43899</v>
+        <v>43913</v>
       </c>
       <c r="AC23" s="5" t="str">
         <f>$I$9</f>
@@ -3356,207 +3276,207 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="AF34:AF35 A32:B32 D32 AA32:XFD32">
-    <cfRule type="cellIs" dxfId="51" priority="132" operator="between">
+    <cfRule type="cellIs" dxfId="43" priority="132" operator="between">
       <formula>$I$11</formula>
       <formula>$I$11</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="50" priority="133" operator="between">
+    <cfRule type="cellIs" dxfId="42" priority="133" operator="between">
       <formula>$I$10</formula>
       <formula>$I$10</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="49" priority="134" operator="between">
+    <cfRule type="cellIs" dxfId="41" priority="134" operator="between">
       <formula>$I$9</formula>
       <formula>$I$9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A20:XFD20">
-    <cfRule type="cellIs" dxfId="48" priority="130" operator="between">
+    <cfRule type="cellIs" dxfId="40" priority="130" operator="between">
       <formula>$K$10</formula>
       <formula>$K$10</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="47" priority="131" operator="between">
+    <cfRule type="cellIs" dxfId="39" priority="131" operator="between">
       <formula>$K$9</formula>
       <formula>$K$9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E35:Z37">
-    <cfRule type="cellIs" dxfId="46" priority="127" operator="between">
+    <cfRule type="cellIs" dxfId="38" priority="127" operator="between">
       <formula>$I$11</formula>
       <formula>$I$11</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="128" operator="between">
+    <cfRule type="cellIs" dxfId="37" priority="128" operator="between">
       <formula>$I$10</formula>
       <formula>$I$10</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="44" priority="129" operator="between">
+    <cfRule type="cellIs" dxfId="36" priority="129" operator="between">
       <formula>$I$9</formula>
       <formula>$I$9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A24:D24 C25:C32 AA24:XFD24">
-    <cfRule type="cellIs" dxfId="43" priority="124" operator="between">
+    <cfRule type="cellIs" dxfId="35" priority="124" operator="between">
       <formula>$I$11</formula>
       <formula>$I$11</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="125" operator="between">
+    <cfRule type="cellIs" dxfId="34" priority="125" operator="between">
       <formula>$I$10</formula>
       <formula>$I$10</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="41" priority="126" operator="between">
+    <cfRule type="cellIs" dxfId="33" priority="126" operator="between">
       <formula>$I$9</formula>
       <formula>$I$9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A25:B25 D25 AA25:XFD25">
-    <cfRule type="cellIs" dxfId="40" priority="121" operator="between">
+    <cfRule type="cellIs" dxfId="32" priority="121" operator="between">
       <formula>$I$11</formula>
       <formula>$I$11</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="39" priority="122" operator="between">
+    <cfRule type="cellIs" dxfId="31" priority="122" operator="between">
       <formula>$I$10</formula>
       <formula>$I$10</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="123" operator="between">
+    <cfRule type="cellIs" dxfId="30" priority="123" operator="between">
       <formula>$I$9</formula>
       <formula>$I$9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A26:B26 D26 AA26:XFD26">
-    <cfRule type="cellIs" dxfId="37" priority="118" operator="between">
+    <cfRule type="cellIs" dxfId="29" priority="118" operator="between">
       <formula>$I$11</formula>
       <formula>$I$11</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="119" operator="between">
+    <cfRule type="cellIs" dxfId="28" priority="119" operator="between">
       <formula>$I$10</formula>
       <formula>$I$10</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="35" priority="120" operator="between">
+    <cfRule type="cellIs" dxfId="27" priority="120" operator="between">
       <formula>$I$9</formula>
       <formula>$I$9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A31:B31 D31 AA31:XFD31">
-    <cfRule type="cellIs" dxfId="34" priority="100" operator="between">
+    <cfRule type="cellIs" dxfId="26" priority="100" operator="between">
       <formula>$I$11</formula>
       <formula>$I$11</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="101" operator="between">
+    <cfRule type="cellIs" dxfId="25" priority="101" operator="between">
       <formula>$I$10</formula>
       <formula>$I$10</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="102" operator="between">
+    <cfRule type="cellIs" dxfId="24" priority="102" operator="between">
       <formula>$I$9</formula>
       <formula>$I$9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A27:B27 D27 AA27:XFD27">
-    <cfRule type="cellIs" dxfId="31" priority="112" operator="between">
+    <cfRule type="cellIs" dxfId="23" priority="112" operator="between">
       <formula>$I$11</formula>
       <formula>$I$11</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="113" operator="between">
+    <cfRule type="cellIs" dxfId="22" priority="113" operator="between">
       <formula>$I$10</formula>
       <formula>$I$10</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="114" operator="between">
+    <cfRule type="cellIs" dxfId="21" priority="114" operator="between">
       <formula>$I$9</formula>
       <formula>$I$9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A28:B28 D28 AA28:XFD28">
-    <cfRule type="cellIs" dxfId="28" priority="109" operator="between">
+    <cfRule type="cellIs" dxfId="20" priority="109" operator="between">
       <formula>$I$11</formula>
       <formula>$I$11</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="110" operator="between">
+    <cfRule type="cellIs" dxfId="19" priority="110" operator="between">
       <formula>$I$10</formula>
       <formula>$I$10</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="111" operator="between">
+    <cfRule type="cellIs" dxfId="18" priority="111" operator="between">
       <formula>$I$9</formula>
       <formula>$I$9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A29:B29 D29 AA29:XFD29">
-    <cfRule type="cellIs" dxfId="25" priority="106" operator="between">
+    <cfRule type="cellIs" dxfId="17" priority="106" operator="between">
       <formula>$I$11</formula>
       <formula>$I$11</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="107" operator="between">
+    <cfRule type="cellIs" dxfId="16" priority="107" operator="between">
       <formula>$I$10</formula>
       <formula>$I$10</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="108" operator="between">
+    <cfRule type="cellIs" dxfId="15" priority="108" operator="between">
       <formula>$I$9</formula>
       <formula>$I$9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A30:B30 D30 AA30:XFD30">
-    <cfRule type="cellIs" dxfId="22" priority="103" operator="between">
+    <cfRule type="cellIs" dxfId="14" priority="103" operator="between">
       <formula>$I$11</formula>
       <formula>$I$11</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="104" operator="between">
+    <cfRule type="cellIs" dxfId="13" priority="104" operator="between">
       <formula>$I$10</formula>
       <formula>$I$10</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="105" operator="between">
+    <cfRule type="cellIs" dxfId="12" priority="105" operator="between">
       <formula>$I$9</formula>
       <formula>$I$9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A33:B33 D33 AA33:XFD33">
-    <cfRule type="cellIs" dxfId="19" priority="97" operator="between">
+    <cfRule type="cellIs" dxfId="11" priority="97" operator="between">
       <formula>$I$11</formula>
       <formula>$I$11</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="98" operator="between">
+    <cfRule type="cellIs" dxfId="10" priority="98" operator="between">
       <formula>$I$10</formula>
       <formula>$I$10</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="99" operator="between">
+    <cfRule type="cellIs" dxfId="9" priority="99" operator="between">
       <formula>$I$9</formula>
       <formula>$I$9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C33">
-    <cfRule type="cellIs" dxfId="16" priority="94" operator="between">
+    <cfRule type="cellIs" dxfId="8" priority="94" operator="between">
       <formula>$I$11</formula>
       <formula>$I$11</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="95" operator="between">
+    <cfRule type="cellIs" dxfId="7" priority="95" operator="between">
       <formula>$I$10</formula>
       <formula>$I$10</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="96" operator="between">
+    <cfRule type="cellIs" dxfId="6" priority="96" operator="between">
       <formula>$I$9</formula>
       <formula>$I$9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P24:Z27">
-    <cfRule type="cellIs" dxfId="8" priority="82" operator="between">
+    <cfRule type="cellIs" dxfId="5" priority="82" operator="between">
       <formula>$I$11</formula>
       <formula>$I$11</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="83" operator="between">
+    <cfRule type="cellIs" dxfId="4" priority="83" operator="between">
       <formula>$I$10</formula>
       <formula>$I$10</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="84" operator="between">
+    <cfRule type="cellIs" dxfId="3" priority="84" operator="between">
       <formula>$I$9</formula>
       <formula>$I$9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E28:Z33 E24:O27">
-    <cfRule type="cellIs" dxfId="11" priority="43" operator="between">
+    <cfRule type="cellIs" dxfId="2" priority="43" operator="between">
       <formula>$I$11</formula>
       <formula>$I$11</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="44" operator="between">
+    <cfRule type="cellIs" dxfId="1" priority="44" operator="between">
       <formula>$I$10</formula>
       <formula>$I$10</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="45" operator="between">
+    <cfRule type="cellIs" dxfId="0" priority="45" operator="between">
       <formula>$I$9</formula>
       <formula>$I$9</formula>
     </cfRule>

</xml_diff>